<commit_message>
Updated test cases and bugs report
</commit_message>
<xml_diff>
--- a/AireLogicTestsCaseBugs.xlsx
+++ b/AireLogicTestsCaseBugs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e-man/Documents/AireLogic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A71B28B-4E83-1C4C-B82B-0645D9D7A0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E327588-E414-0443-907B-94906E2D6685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Some more tests" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="127">
   <si>
     <t>Test Cases</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>If a user enters an existing username and clicks Start, The Game resets all the fields to 0</t>
+  </si>
+  <si>
+    <t>Attachments</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -662,28 +665,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1363,8 +1354,8 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -1382,32 +1373,32 @@
     <col min="10" max="16384" width="12.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+      <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="16" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1427,10 +1418,10 @@
       <c r="E2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.15">
       <c r="B3" s="9"/>
@@ -1439,10 +1430,10 @@
       <c r="E3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.15">
       <c r="B4" s="9"/>
@@ -1451,41 +1442,41 @@
       <c r="E4" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.15">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" ht="147" x14ac:dyDescent="0.15">
       <c r="B8" s="9" t="s">
@@ -1500,7 +1491,7 @@
       <c r="E8" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1520,7 +1511,7 @@
       <c r="E10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="9" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1542,15 +1533,15 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="22"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" ht="147" x14ac:dyDescent="0.15">
       <c r="B14" s="9" t="s">
@@ -1565,7 +1556,7 @@
       <c r="E14" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1585,43 +1576,43 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-    </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="1:9" ht="84" x14ac:dyDescent="0.15">
       <c r="B18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="9"/>
@@ -1633,7 +1624,7 @@
       <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.15">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C23" s="9"/>
@@ -1763,12 +1754,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842FB117-103E-C040-B677-9482B8BB7071}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.15"/>
@@ -1781,10 +1772,12 @@
     <col min="7" max="7" width="57.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="53.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="77" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="4"/>
+    <col min="10" max="11" width="10.83203125" style="4"/>
+    <col min="12" max="12" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -1810,18 +1803,24 @@
         <v>12</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="L1" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1830,7 +1829,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="168" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="168" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1856,7 +1855,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="84" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1888,7 +1887,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="231" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="231" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>50</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1920,7 +1919,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="147" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="147" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1952,7 +1951,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="210" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="210" x14ac:dyDescent="0.15">
       <c r="B13" s="9" t="s">
         <v>49</v>
       </c>
@@ -1975,7 +1974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1984,8 +1983,8 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:10" s="10" customFormat="1" ht="189" x14ac:dyDescent="0.15">
-      <c r="B15" s="11" t="s">
+    <row r="15" spans="1:12" ht="189" x14ac:dyDescent="0.15">
+      <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -2000,14 +1999,14 @@
       <c r="F15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2016,11 +2015,11 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" s="13" customFormat="1" ht="258" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" s="11" customFormat="1" ht="258" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -2048,11 +2047,11 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:8" s="13" customFormat="1" ht="147" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:8" s="11" customFormat="1" ht="147" x14ac:dyDescent="0.15">
       <c r="B19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -2064,27 +2063,27 @@
       <c r="F19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="9" t="s">
         <v>58</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="16" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="2:8" s="17" customFormat="1" ht="232" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="14" t="s">
+    <row r="20" spans="2:8" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="2:8" s="11" customFormat="1" ht="232" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -2096,10 +2095,10 @@
       <c r="F21" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2115,7 +2114,7 @@
       <c r="B23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -2135,7 +2134,7 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="21" x14ac:dyDescent="0.15">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="14" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2160,7 +2159,7 @@
       </c>
     </row>
     <row r="34" spans="2:2" ht="21" x14ac:dyDescent="0.15">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="14" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>